<commit_message>
fixed #1 and #10
</commit_message>
<xml_diff>
--- a/data/last-authors-list_2024-08-08_worked.xlsx
+++ b/data/last-authors-list_2024-08-08_worked.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giandomenicobisaccia/VS/CMR-publications-dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97060746-7E5D-674B-996E-EA4913083C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF737122-4975-2049-9ABD-E5CBCFCE6FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,780 +20,786 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="258">
-  <si>
-    <t>last_authors_cmr_list</t>
-  </si>
-  <si>
-    <t>PETERSEN, STEFFEN E</t>
-  </si>
-  <si>
-    <t>TAYLOR, ANDREW J</t>
-  </si>
-  <si>
-    <t>KWONG, RAYMOND Y</t>
-  </si>
-  <si>
-    <t>YANG, ZHI-GANG</t>
-  </si>
-  <si>
-    <t>LIU, HUI</t>
-  </si>
-  <si>
-    <t>LI, YUAN</t>
-  </si>
-  <si>
-    <t>XU, LEI</t>
-  </si>
-  <si>
-    <t>REINSTADLER, SEBASTIAN J</t>
-  </si>
-  <si>
-    <t>MERLO, MARCO</t>
-  </si>
-  <si>
-    <t>WANG, YINING</t>
-  </si>
-  <si>
-    <t>ZHAO, SHIHUA</t>
-  </si>
-  <si>
-    <t>LURZ, PHILIPP</t>
-  </si>
-  <si>
-    <t>COOPER, LESLIE T</t>
-  </si>
-  <si>
-    <t>MULLER, STEVEN A</t>
-  </si>
-  <si>
-    <t>CAPTUR, GABRIELLA</t>
-  </si>
-  <si>
-    <t>PANDEY, AMBARISH</t>
-  </si>
-  <si>
-    <t>CIPRIANI, ALBERTO</t>
-  </si>
-  <si>
-    <t>CHEN, YUCHENG</t>
-  </si>
-  <si>
-    <t>ROWIN, ETHAN J</t>
-  </si>
-  <si>
-    <t>FONTANA, MARIANNA</t>
-  </si>
-  <si>
-    <t>OLMOS, CARMEN</t>
-  </si>
-  <si>
-    <t>SCHOENNAGEL, BJOERN P</t>
-  </si>
-  <si>
-    <t>WU, LIAN-MING</t>
-  </si>
-  <si>
-    <t>ZHONG, YUMIN</t>
-  </si>
-  <si>
-    <t>LIMA, JOÃO A C</t>
-  </si>
-  <si>
-    <t>LI, JIANG</t>
-  </si>
-  <si>
-    <t>SUN, JIAYU</t>
-  </si>
-  <si>
-    <t>PARK, CHUL HWAN</t>
-  </si>
-  <si>
-    <t>CHEN, HANG</t>
-  </si>
-  <si>
-    <t>LU, MINJIE</t>
-  </si>
-  <si>
-    <t>WANG, XI-MING</t>
-  </si>
-  <si>
-    <t>MITSOURAS, DIMITRIOS</t>
-  </si>
-  <si>
-    <t>PRASAD, SANJAY K</t>
-  </si>
-  <si>
-    <t>MYUNG, SEUNG-JAE</t>
-  </si>
-  <si>
-    <t>DHARMAKUMAR, ROHAN</t>
-  </si>
-  <si>
-    <t>SINN, MARTIN</t>
-  </si>
-  <si>
-    <t>HUANG, YULI</t>
-  </si>
-  <si>
-    <t>SABA, LUCA</t>
-  </si>
-  <si>
-    <t>YANG, MIN-FU</t>
-  </si>
-  <si>
-    <t>HIRAI, TOSHINORI</t>
-  </si>
-  <si>
-    <t>BLASZCZYK, EDYTA</t>
-  </si>
-  <si>
-    <t>REITER, URSULA</t>
-  </si>
-  <si>
-    <t>PENG, LIQING</t>
-  </si>
-  <si>
-    <t>YANG, GUI FEN</t>
-  </si>
-  <si>
-    <t>LI, TAO</t>
-  </si>
-  <si>
-    <t>TAHIR, ENVER</t>
-  </si>
-  <si>
-    <t>YAO, WEIWU</t>
-  </si>
-  <si>
-    <t>PONTANA, FRANÇOIS</t>
-  </si>
-  <si>
-    <t>BUCCIARELLI-DUCCI, CHIARA</t>
-  </si>
-  <si>
-    <t>LEE, JI WON</t>
-  </si>
-  <si>
-    <t>NEZAFAT, REZA</t>
-  </si>
-  <si>
-    <t>OMIDI, NEGAR</t>
-  </si>
-  <si>
-    <t>FRIEDBERG, MARK K</t>
-  </si>
-  <si>
-    <t>MEUCCI, MARIA CHIARA</t>
-  </si>
-  <si>
-    <t>ZHANG, LONG JIANG</t>
-  </si>
-  <si>
-    <t>FISCHER, KADY</t>
-  </si>
-  <si>
-    <t>CHOI, BYOUNG WOOK</t>
-  </si>
-  <si>
-    <t>LINK, MARK S</t>
-  </si>
-  <si>
-    <t>WINTERSPERGER, BERND J</t>
-  </si>
-  <si>
-    <t>LUETKENS, JULIAN A</t>
-  </si>
-  <si>
-    <t>SCHWITTER, JUERG</t>
-  </si>
-  <si>
-    <t>TANG, GUANGYU</t>
-  </si>
-  <si>
-    <t>GRÄNI, CHRISTOPH</t>
-  </si>
-  <si>
-    <t>NERI, EMANUELE</t>
-  </si>
-  <si>
-    <t>AVANESOV, MAXIM</t>
-  </si>
-  <si>
-    <t>JUAN, YU-HSIANG</t>
-  </si>
-  <si>
-    <t>COCHET, HUBERT</t>
-  </si>
-  <si>
-    <t>XIE, MINGXING</t>
-  </si>
-  <si>
-    <t>ABDELRAHMAN, AHMED S</t>
-  </si>
-  <si>
-    <t>JEROSCH-HEROLD, MICHAEL</t>
-  </si>
-  <si>
-    <t>HU, HONGJIE</t>
-  </si>
-  <si>
-    <t>NEWBY, DAVID E</t>
-  </si>
-  <si>
-    <t>MARKL, MICHAEL</t>
-  </si>
-  <si>
-    <t>KOROSOGLOU, GRIGORIOS</t>
-  </si>
-  <si>
-    <t>FERREIRA, VANESSA M</t>
-  </si>
-  <si>
-    <t>SHENOY, CHETAN</t>
-  </si>
-  <si>
-    <t>CADEMARTIRI, FILIPPO</t>
-  </si>
-  <si>
-    <t>LIMONGELLI, GIUSEPPE</t>
-  </si>
-  <si>
-    <t>KORANTZOPOULOS, PANAGIOTIS</t>
-  </si>
-  <si>
-    <t>KAASALAINEN, TOUKO</t>
-  </si>
-  <si>
-    <t>MAYR, AGNES</t>
-  </si>
-  <si>
-    <t>PU, JUN</t>
-  </si>
-  <si>
-    <t>JIN, HANG</t>
-  </si>
-  <si>
-    <t>YANG, WENJIE</t>
-  </si>
-  <si>
-    <t>BARISON, ANDREA</t>
-  </si>
-  <si>
-    <t>GARCÍA-PAVÍA, PABLO</t>
-  </si>
-  <si>
-    <t>AL-MALLAH, MOUAZ H</t>
-  </si>
-  <si>
-    <t>THUNY, FRANCK</t>
-  </si>
-  <si>
-    <t>YANG, DONG HYUN</t>
-  </si>
-  <si>
-    <t>QIU, TIAN</t>
-  </si>
-  <si>
-    <t>WIEBEN, OLIVER</t>
-  </si>
-  <si>
-    <t>HANNEMAN, KATE</t>
-  </si>
-  <si>
-    <t>MOON, JAMES</t>
-  </si>
-  <si>
-    <t>ZHOU, PENG</t>
-  </si>
-  <si>
-    <t>HENEIN, MICHAEL Y</t>
-  </si>
-  <si>
-    <t>PEPE, ALESSIA</t>
-  </si>
-  <si>
-    <t>MELONI, ANTONELLA</t>
-  </si>
-  <si>
-    <t>NEWBURGER, JANE W</t>
-  </si>
-  <si>
-    <t>ULM, BARBARA</t>
-  </si>
-  <si>
-    <t>SONG, LEI</t>
-  </si>
-  <si>
-    <t>PENNELL, DUDLEY J</t>
-  </si>
-  <si>
-    <t>BODI, VICENTE</t>
-  </si>
-  <si>
-    <t>KRAMER, CHRISTOPHER M</t>
-  </si>
-  <si>
-    <t>HASHMI, ARSALAN TALIB</t>
-  </si>
-  <si>
-    <t>DE ROOS, ALBERT</t>
-  </si>
-  <si>
-    <t>ARAI, ANDREW E</t>
-  </si>
-  <si>
-    <t>YAN, ANDREW T</t>
-  </si>
-  <si>
-    <t>MARCHLINSKI, FRANCIS E</t>
-  </si>
-  <si>
-    <t>BAUCE, BARBARA</t>
-  </si>
-  <si>
-    <t>KIM, RAYMOND J</t>
-  </si>
-  <si>
-    <t>LUND, GUNNAR K</t>
-  </si>
-  <si>
-    <t>LI, ZHEN-LIN</t>
-  </si>
-  <si>
-    <t>CHEUNG, JIM W</t>
-  </si>
-  <si>
-    <t>WILLEMS, RIK</t>
-  </si>
-  <si>
-    <t>LEE, SEUNG-PYO</t>
-  </si>
-  <si>
-    <t>HAÏSSAGUERRE, MICHEL</t>
-  </si>
-  <si>
-    <t>LANZ, JONAS</t>
-  </si>
-  <si>
-    <t>LEHTONEN, JUKKA</t>
-  </si>
-  <si>
-    <t>NICHOLLS, MARK</t>
-  </si>
-  <si>
-    <t>DOHI, KAORU</t>
-  </si>
-  <si>
-    <t>PETRIE, MARK C</t>
-  </si>
-  <si>
-    <t>VASANAWALA, SHREYAS S</t>
-  </si>
-  <si>
-    <t>SCHMITT, MATTHIAS</t>
-  </si>
-  <si>
-    <t>FERREIRA-GONZÁLEZ, IGNACIO</t>
-  </si>
-  <si>
-    <t>RINK, LAWRENCE D</t>
-  </si>
-  <si>
-    <t>VASSILIKOS, VASSILIOS P</t>
-  </si>
-  <si>
-    <t>CARRIERE, KEUMHEE C</t>
-  </si>
-  <si>
-    <t>HAZEBROEK, MARK R</t>
-  </si>
-  <si>
-    <t>ROCA-LUQUE, IVO</t>
-  </si>
-  <si>
-    <t>FALETTI, RICCARDO</t>
-  </si>
-  <si>
-    <t>BENGEL, FRANK M</t>
-  </si>
-  <si>
-    <t>SITGES, MARTA</t>
-  </si>
-  <si>
-    <t>EMRICH, TILMAN</t>
-  </si>
-  <si>
-    <t>ROMANO, GIUSEPPE</t>
-  </si>
-  <si>
-    <t>SHARMA, SANJIV</t>
-  </si>
-  <si>
-    <t>KOVACS, RICHARD</t>
-  </si>
-  <si>
-    <t>MOON, JAMES C</t>
-  </si>
-  <si>
-    <t>JENSEN, JAMES A</t>
-  </si>
-  <si>
-    <t>CREA, FILIPPO</t>
-  </si>
-  <si>
-    <t>PAPAVASSILIU, THEANO</t>
-  </si>
-  <si>
-    <t>GARCÍA-DORADO, DAVID</t>
-  </si>
-  <si>
-    <t>ZAMORANO, JOSE LUIS</t>
-  </si>
-  <si>
-    <t>MA, XIAOHAI</t>
-  </si>
-  <si>
-    <t>LEYVA, FRANCISCO</t>
-  </si>
-  <si>
-    <t>HOU, YANG</t>
-  </si>
-  <si>
-    <t>LINDNER, JONATHAN R</t>
-  </si>
-  <si>
-    <t>AKHTER, NAUSHEEN</t>
-  </si>
-  <si>
-    <t>TONDO, CLAUDIO</t>
-  </si>
-  <si>
-    <t>TUNG, RODERICK</t>
-  </si>
-  <si>
-    <t>LIU, KAN</t>
-  </si>
-  <si>
-    <t>SCHULZ-MENGER, JEANETTE</t>
-  </si>
-  <si>
-    <t>TIAN, JIE</t>
-  </si>
-  <si>
-    <t>HWANG, SUNG HO</t>
-  </si>
-  <si>
-    <t>PACKER, DOUGLAS L</t>
-  </si>
-  <si>
-    <t>JACOBY, DANIEL</t>
-  </si>
-  <si>
-    <t>SINGH, ANVESHA</t>
-  </si>
-  <si>
-    <t>MOLLAZADEH, REZA</t>
-  </si>
-  <si>
-    <t>MADSEN, PER LAV</t>
-  </si>
-  <si>
-    <t>D'ASCENZI, FLAVIO</t>
-  </si>
-  <si>
-    <t>JUDSON, MARC A</t>
-  </si>
-  <si>
-    <t>KARAARSLAN, ERCAN</t>
-  </si>
-  <si>
-    <t>BOGAERT, JAN</t>
-  </si>
-  <si>
-    <t>FUSTER, VALENTÍN</t>
-  </si>
-  <si>
-    <t>REZAEIAN, NAHID</t>
-  </si>
-  <si>
-    <t>HALUSHKA, MARC K</t>
-  </si>
-  <si>
-    <t>TRIVIERI, MARIA G</t>
-  </si>
-  <si>
-    <t>OH, JAE K</t>
-  </si>
-  <si>
-    <t>MASCI, PIER GIORGIO</t>
-  </si>
-  <si>
-    <t>SIANOS, G</t>
-  </si>
-  <si>
-    <t>SHAH, DIPAN J</t>
-  </si>
-  <si>
-    <t>GREEN, ULRIKA BIRGERSDOTTER</t>
-  </si>
-  <si>
-    <t>XIA, LIMING</t>
-  </si>
-  <si>
-    <t>JACQUIER, A</t>
-  </si>
-  <si>
-    <t>WANN, L SAMUEL</t>
-  </si>
-  <si>
-    <t>PONTONE, GIANLUCA</t>
-  </si>
-  <si>
-    <t>MCNAMARA, DAVID A</t>
-  </si>
-  <si>
-    <t>GUO, YINGKUN</t>
-  </si>
-  <si>
-    <t>BOGUN, FRANK</t>
-  </si>
-  <si>
-    <t>KIM, TAE HOON</t>
-  </si>
-  <si>
-    <t>MOJIBIAN, HAMID</t>
-  </si>
-  <si>
-    <t>BEGHETTI, MAURICE</t>
-  </si>
-  <si>
-    <t>IBANEZ, BORJA</t>
-  </si>
-  <si>
-    <t>WANG, KEZHENG</t>
-  </si>
-  <si>
-    <t>EMDIN, MICHELE</t>
-  </si>
-  <si>
-    <t>SINAGRA, GIANFRANCO</t>
-  </si>
-  <si>
-    <t>WANG, MEIYUN</t>
-  </si>
-  <si>
-    <t>CHANDRASHEKHAR, Y</t>
-  </si>
-  <si>
-    <t>GROGAN, MARTHA</t>
-  </si>
-  <si>
-    <t>PILZ, GÜNTER</t>
-  </si>
-  <si>
-    <t>MANKA, ROBERT</t>
-  </si>
-  <si>
-    <t>BEYGUI, FARZIN</t>
-  </si>
-  <si>
-    <t>GAO, FABAO</t>
-  </si>
-  <si>
-    <t>ATALAY, MICHAEL K</t>
-  </si>
-  <si>
-    <t>STONE, GREGG W</t>
-  </si>
-  <si>
-    <t>HSIAO, ALBERT</t>
-  </si>
-  <si>
-    <t>MANDOUR, KHALED</t>
-  </si>
-  <si>
-    <t>LIANG, BO</t>
-  </si>
-  <si>
-    <t>HAGIWARA, NOBUHISA</t>
-  </si>
-  <si>
-    <t>XU, BO</t>
-  </si>
-  <si>
-    <t>MANCIA, GIUSEPPE</t>
-  </si>
-  <si>
-    <t>MCCANN, GERRY P</t>
-  </si>
-  <si>
-    <t>NEILAN, TOMAS G</t>
-  </si>
-  <si>
-    <t>ZHONG, LIANG</t>
-  </si>
-  <si>
-    <t>LEE, SEUNG PYO</t>
-  </si>
-  <si>
-    <t>BERRY, COLIN</t>
-  </si>
-  <si>
-    <t>SIEGEL, ROBERT J</t>
-  </si>
-  <si>
-    <t>DWECK, MARC R</t>
-  </si>
-  <si>
-    <t>BAYÉS-GENÍS, ANTONI</t>
-  </si>
-  <si>
-    <t>LEE, BAE YOUNG</t>
-  </si>
-  <si>
-    <t>RODRÍGUEZ-PALOMARES, JOSÉ F</t>
-  </si>
-  <si>
-    <t>CAMELI, MATTEO</t>
-  </si>
-  <si>
-    <t>NOUTSIAS, MICHEL</t>
-  </si>
-  <si>
-    <t>TEMPLIN, CHRISTIAN</t>
-  </si>
-  <si>
-    <t>DI BELLA, GIANLUCA</t>
-  </si>
-  <si>
-    <t>MARINO, PAOLO</t>
-  </si>
-  <si>
-    <t>COSYNS, BERNARD</t>
-  </si>
-  <si>
-    <t>YONG, HWAN SEOK</t>
-  </si>
-  <si>
-    <t>TRAYANOVA, NATALIA A</t>
-  </si>
-  <si>
-    <t>SIMONETTI, ORLANDO P</t>
-  </si>
-  <si>
-    <t>KERKAR, PRAFULLA</t>
-  </si>
-  <si>
-    <t>SALGADO, RODRIGO</t>
-  </si>
-  <si>
-    <t>CONNELLY, KIM A</t>
-  </si>
-  <si>
-    <t>VAGO, HAJNALKA</t>
-  </si>
-  <si>
-    <t>JADDOE, VINCENT WV</t>
-  </si>
-  <si>
-    <t>YOO, SHI JOON</t>
-  </si>
-  <si>
-    <t>NISHTALA, ARVIND</t>
-  </si>
-  <si>
-    <t>ARYA, ARASH</t>
-  </si>
-  <si>
-    <t>LIM, PHANG BOON</t>
-  </si>
-  <si>
-    <t>EVANGELISTA, ARTURO</t>
-  </si>
-  <si>
-    <t>WATKINS, HUGH</t>
-  </si>
-  <si>
-    <t>GUTBERLET, MATTHIAS</t>
-  </si>
-  <si>
-    <t>LEINER, TIM</t>
-  </si>
-  <si>
-    <t>FIRMIN, DAVID</t>
-  </si>
-  <si>
-    <t>NIEDERER, STEVEN A</t>
-  </si>
-  <si>
-    <t>FRANKEL, DAVID S</t>
-  </si>
-  <si>
-    <t>ROEST, ARNO A W</t>
-  </si>
-  <si>
-    <t>WINDECKER, STEPHAN</t>
-  </si>
-  <si>
-    <t>MORISHIMA, ITSURO</t>
-  </si>
-  <si>
-    <t>RINALDI, CHRISTOPHER A</t>
-  </si>
-  <si>
-    <t>KACHENOURA, NADJIA</t>
-  </si>
-  <si>
-    <t>BHATT, DEEPAK L</t>
-  </si>
-  <si>
-    <t>HONDA, HIROSHI</t>
-  </si>
-  <si>
-    <t>WEI, MENG</t>
-  </si>
-  <si>
-    <t>ZENG, MENGSU</t>
-  </si>
-  <si>
-    <t>LÜSCHER, THOMAS F</t>
-  </si>
-  <si>
-    <t>O'NEILL, WILLIAM W</t>
-  </si>
-  <si>
-    <t>VAN ROYEN, NIELS</t>
-  </si>
-  <si>
-    <t>BLUEMKE, DAVID A</t>
-  </si>
-  <si>
-    <t>FRANCONE, MARCO</t>
-  </si>
-  <si>
-    <t>KHANJI, MOHAMMED Y</t>
-  </si>
-  <si>
-    <t>LA GERCHE, ANDRÉ</t>
-  </si>
-  <si>
-    <t>WESTENBERG, JOS J M</t>
-  </si>
-  <si>
-    <t>WONG, RAYMOND CHING-CHEW</t>
-  </si>
-  <si>
-    <t>VAN DER GEEST, ROB J</t>
-  </si>
-  <si>
-    <t>WILDE, ARTHUR A M</t>
-  </si>
-  <si>
-    <t>AQUARO, GIOVANNI DONATO</t>
-  </si>
-  <si>
-    <t>BEZZINA, CONNIE R</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="260">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>STEFFEN E PETERSEN</t>
+  </si>
+  <si>
+    <t>ANDREW J TAYLOR</t>
+  </si>
+  <si>
+    <t>RAYMOND Y KWONG</t>
+  </si>
+  <si>
+    <t>ZHI-GANG YANG</t>
+  </si>
+  <si>
+    <t>HUI LIU</t>
+  </si>
+  <si>
+    <t>YUAN LI</t>
+  </si>
+  <si>
+    <t>LEI XU</t>
+  </si>
+  <si>
+    <t>SEBASTIAN J REINSTADLER</t>
+  </si>
+  <si>
+    <t>MARCO MERLO</t>
+  </si>
+  <si>
+    <t>YINING WANG</t>
+  </si>
+  <si>
+    <t>SHIHUA ZHAO</t>
+  </si>
+  <si>
+    <t>PHILIPP LURZ</t>
+  </si>
+  <si>
+    <t>LESLIE T COOPER</t>
+  </si>
+  <si>
+    <t>STEVEN A MULLER</t>
+  </si>
+  <si>
+    <t>GABRIELLA CAPTUR</t>
+  </si>
+  <si>
+    <t>AMBARISH PANDEY</t>
+  </si>
+  <si>
+    <t>ALBERTO CIPRIANI</t>
+  </si>
+  <si>
+    <t>YUCHENG CHEN</t>
+  </si>
+  <si>
+    <t>ETHAN J ROWIN</t>
+  </si>
+  <si>
+    <t>MARIANNA FONTANA</t>
+  </si>
+  <si>
+    <t>CARMEN OLMOS</t>
+  </si>
+  <si>
+    <t>BJOERN P SCHOENNAGEL</t>
+  </si>
+  <si>
+    <t>LIAN-MING WU</t>
+  </si>
+  <si>
+    <t>YUMIN ZHONG</t>
+  </si>
+  <si>
+    <t>JOÃO A C LIMA</t>
+  </si>
+  <si>
+    <t>JIANG LI</t>
+  </si>
+  <si>
+    <t>JIAYU SUN</t>
+  </si>
+  <si>
+    <t>CHUL HWAN PARK</t>
+  </si>
+  <si>
+    <t>HANG CHEN</t>
+  </si>
+  <si>
+    <t>MINJIE LU</t>
+  </si>
+  <si>
+    <t>XI-MING WANG</t>
+  </si>
+  <si>
+    <t>DIMITRIOS MITSOURAS</t>
+  </si>
+  <si>
+    <t>SANJAY K PRASAD</t>
+  </si>
+  <si>
+    <t>SEUNG-JAE MYUNG</t>
+  </si>
+  <si>
+    <t>ROHAN DHARMAKUMAR</t>
+  </si>
+  <si>
+    <t>MARTIN SINN</t>
+  </si>
+  <si>
+    <t>YULI HUANG</t>
+  </si>
+  <si>
+    <t>LUCA SABA</t>
+  </si>
+  <si>
+    <t>MIN-FU YANG</t>
+  </si>
+  <si>
+    <t>TOSHINORI HIRAI</t>
+  </si>
+  <si>
+    <t>EDYTA BLASZCZYK</t>
+  </si>
+  <si>
+    <t>URSULA REITER</t>
+  </si>
+  <si>
+    <t>LIQING PENG</t>
+  </si>
+  <si>
+    <t>GUI FEN YANG</t>
+  </si>
+  <si>
+    <t>TAO LI</t>
+  </si>
+  <si>
+    <t>ENVER TAHIR</t>
+  </si>
+  <si>
+    <t>WEIWU YAO</t>
+  </si>
+  <si>
+    <t>FRANÇOIS PONTANA</t>
+  </si>
+  <si>
+    <t>CHIARA BUCCIARELLI-DUCCI</t>
+  </si>
+  <si>
+    <t>JI WON LEE</t>
+  </si>
+  <si>
+    <t>REZA NEZAFAT</t>
+  </si>
+  <si>
+    <t>NEGAR OMIDI</t>
+  </si>
+  <si>
+    <t>MARK K FRIEDBERG</t>
+  </si>
+  <si>
+    <t>MARIA CHIARA MEUCCI</t>
+  </si>
+  <si>
+    <t>LONG JIANG ZHANG</t>
+  </si>
+  <si>
+    <t>KADY FISCHER</t>
+  </si>
+  <si>
+    <t>BYOUNG WOOK CHOI</t>
+  </si>
+  <si>
+    <t>MARK S LINK</t>
+  </si>
+  <si>
+    <t>BERND J WINTERSPERGER</t>
+  </si>
+  <si>
+    <t>JULIAN A LUETKENS</t>
+  </si>
+  <si>
+    <t>JUERG SCHWITTER</t>
+  </si>
+  <si>
+    <t>GUANGYU TANG</t>
+  </si>
+  <si>
+    <t>CHRISTOPH GRÄNI</t>
+  </si>
+  <si>
+    <t>EMANUELE NERI</t>
+  </si>
+  <si>
+    <t>MAXIM AVANESOV</t>
+  </si>
+  <si>
+    <t>YU-HSIANG JUAN</t>
+  </si>
+  <si>
+    <t>HUBERT COCHET</t>
+  </si>
+  <si>
+    <t>MINGXING XIE</t>
+  </si>
+  <si>
+    <t>AHMED S ABDELRAHMAN</t>
+  </si>
+  <si>
+    <t>MICHAEL JEROSCH-HEROLD</t>
+  </si>
+  <si>
+    <t>HONGJIE HU</t>
+  </si>
+  <si>
+    <t>DAVID E NEWBY</t>
+  </si>
+  <si>
+    <t>MICHAEL MARKL</t>
+  </si>
+  <si>
+    <t>GRIGORIOS KOROSOGLOU</t>
+  </si>
+  <si>
+    <t>VANESSA M FERREIRA</t>
+  </si>
+  <si>
+    <t>CHETAN SHENOY</t>
+  </si>
+  <si>
+    <t>FILIPPO CADEMARTIRI</t>
+  </si>
+  <si>
+    <t>GIUSEPPE LIMONGELLI</t>
+  </si>
+  <si>
+    <t>PANAGIOTIS KORANTZOPOULOS</t>
+  </si>
+  <si>
+    <t>TOUKO KAASALAINEN</t>
+  </si>
+  <si>
+    <t>AGNES MAYR</t>
+  </si>
+  <si>
+    <t>JUN PU</t>
+  </si>
+  <si>
+    <t>HANG JIN</t>
+  </si>
+  <si>
+    <t>WENJIE YANG</t>
+  </si>
+  <si>
+    <t>ANDREA BARISON</t>
+  </si>
+  <si>
+    <t>PABLO GARCÍA-PAVÍA</t>
+  </si>
+  <si>
+    <t>MOUAZ H AL-MALLAH</t>
+  </si>
+  <si>
+    <t>FRANCK THUNY</t>
+  </si>
+  <si>
+    <t>DONG HYUN YANG</t>
+  </si>
+  <si>
+    <t>TIAN QIU</t>
+  </si>
+  <si>
+    <t>OLIVER WIEBEN</t>
+  </si>
+  <si>
+    <t>KATE HANNEMAN</t>
+  </si>
+  <si>
+    <t>JAMES MOON</t>
+  </si>
+  <si>
+    <t>PENG ZHOU</t>
+  </si>
+  <si>
+    <t>MICHAEL Y HENEIN</t>
+  </si>
+  <si>
+    <t>ALESSIA PEPE</t>
+  </si>
+  <si>
+    <t>ANTONELLA MELONI</t>
+  </si>
+  <si>
+    <t>JANE W NEWBURGER</t>
+  </si>
+  <si>
+    <t>BARBARA ULM</t>
+  </si>
+  <si>
+    <t>LEI SONG</t>
+  </si>
+  <si>
+    <t>DUDLEY J PENNELL</t>
+  </si>
+  <si>
+    <t>VICENTE BODI</t>
+  </si>
+  <si>
+    <t>CHRISTOPHER M KRAMER</t>
+  </si>
+  <si>
+    <t>ARSALAN TALIB HASHMI</t>
+  </si>
+  <si>
+    <t>ALBERT DE ROOS</t>
+  </si>
+  <si>
+    <t>ANDREW E ARAI</t>
+  </si>
+  <si>
+    <t>ANDREW T YAN</t>
+  </si>
+  <si>
+    <t>FRANCIS E MARCHLINSKI</t>
+  </si>
+  <si>
+    <t>BARBARA BAUCE</t>
+  </si>
+  <si>
+    <t>RAYMOND J KIM</t>
+  </si>
+  <si>
+    <t>GUNNAR K LUND</t>
+  </si>
+  <si>
+    <t>ZHEN-LIN LI</t>
+  </si>
+  <si>
+    <t>JIM W CHEUNG</t>
+  </si>
+  <si>
+    <t>RIK WILLEMS</t>
+  </si>
+  <si>
+    <t>SEUNG-PYO LEE</t>
+  </si>
+  <si>
+    <t>MICHEL HAÏSSAGUERRE</t>
+  </si>
+  <si>
+    <t>JONAS LANZ</t>
+  </si>
+  <si>
+    <t>JUKKA LEHTONEN</t>
+  </si>
+  <si>
+    <t>MARK NICHOLLS</t>
+  </si>
+  <si>
+    <t>KAORU DOHI</t>
+  </si>
+  <si>
+    <t>MARK C PETRIE</t>
+  </si>
+  <si>
+    <t>SHREYAS S VASANAWALA</t>
+  </si>
+  <si>
+    <t>MATTHIAS SCHMITT</t>
+  </si>
+  <si>
+    <t>IGNACIO FERREIRA-GONZÁLEZ</t>
+  </si>
+  <si>
+    <t>LAWRENCE D RINK</t>
+  </si>
+  <si>
+    <t>VASSILIOS P VASSILIKOS</t>
+  </si>
+  <si>
+    <t>KEUMHEE C CARRIERE</t>
+  </si>
+  <si>
+    <t>MARK R HAZEBROEK</t>
+  </si>
+  <si>
+    <t>IVO ROCA-LUQUE</t>
+  </si>
+  <si>
+    <t>RICCARDO FALETTI</t>
+  </si>
+  <si>
+    <t>FRANK M BENGEL</t>
+  </si>
+  <si>
+    <t>MARTA SITGES</t>
+  </si>
+  <si>
+    <t>TILMAN EMRICH</t>
+  </si>
+  <si>
+    <t>GIUSEPPE ROMANO</t>
+  </si>
+  <si>
+    <t>SANJIV SHARMA</t>
+  </si>
+  <si>
+    <t>RICHARD KOVACS</t>
+  </si>
+  <si>
+    <t>JAMES C MOON</t>
+  </si>
+  <si>
+    <t>JAMES A JENSEN</t>
+  </si>
+  <si>
+    <t>FILIPPO CREA</t>
+  </si>
+  <si>
+    <t>THEANO PAPAVASSILIU</t>
+  </si>
+  <si>
+    <t>DAVID GARCÍA-DORADO</t>
+  </si>
+  <si>
+    <t>JOSE LUIS ZAMORANO</t>
+  </si>
+  <si>
+    <t>XIAOHAI MA</t>
+  </si>
+  <si>
+    <t>FRANCISCO LEYVA</t>
+  </si>
+  <si>
+    <t>YANG HOU</t>
+  </si>
+  <si>
+    <t>JONATHAN R LINDNER</t>
+  </si>
+  <si>
+    <t>NAUSHEEN AKHTER</t>
+  </si>
+  <si>
+    <t>CLAUDIO TONDO</t>
+  </si>
+  <si>
+    <t>RODERICK TUNG</t>
+  </si>
+  <si>
+    <t>KAN LIU</t>
+  </si>
+  <si>
+    <t>JEANETTE SCHULZ-MENGER</t>
+  </si>
+  <si>
+    <t>JIE TIAN</t>
+  </si>
+  <si>
+    <t>SUNG HO HWANG</t>
+  </si>
+  <si>
+    <t>DOUGLAS L PACKER</t>
+  </si>
+  <si>
+    <t>DANIEL JACOBY</t>
+  </si>
+  <si>
+    <t>ANVESHA SINGH</t>
+  </si>
+  <si>
+    <t>REZA MOLLAZADEH</t>
+  </si>
+  <si>
+    <t>PER LAV MADSEN</t>
+  </si>
+  <si>
+    <t>FLAVIO D'ASCENZI</t>
+  </si>
+  <si>
+    <t>MARC A JUDSON</t>
+  </si>
+  <si>
+    <t>ERCAN KARAARSLAN</t>
+  </si>
+  <si>
+    <t>JAN BOGAERT</t>
+  </si>
+  <si>
+    <t>VALENTÍN FUSTER</t>
+  </si>
+  <si>
+    <t>NAHID REZAEIAN</t>
+  </si>
+  <si>
+    <t>MARC K HALUSHKA</t>
+  </si>
+  <si>
+    <t>MARIA G TRIVIERI</t>
+  </si>
+  <si>
+    <t>JAE K OH</t>
+  </si>
+  <si>
+    <t>PIER GIORGIO MASCI</t>
+  </si>
+  <si>
+    <t>G SIANOS</t>
+  </si>
+  <si>
+    <t>DIPAN J SHAH</t>
+  </si>
+  <si>
+    <t>ULRIKA BIRGERSDOTTER GREEN</t>
+  </si>
+  <si>
+    <t>LIMING XIA</t>
+  </si>
+  <si>
+    <t>A JACQUIER</t>
+  </si>
+  <si>
+    <t>L SAMUEL WANN</t>
+  </si>
+  <si>
+    <t>GIANLUCA PONTONE</t>
+  </si>
+  <si>
+    <t>DAVID A MCNAMARA</t>
+  </si>
+  <si>
+    <t>YINGKUN GUO</t>
+  </si>
+  <si>
+    <t>FRANK BOGUN</t>
+  </si>
+  <si>
+    <t>TAE HOON KIM</t>
+  </si>
+  <si>
+    <t>HAMID MOJIBIAN</t>
+  </si>
+  <si>
+    <t>MAURICE BEGHETTI</t>
+  </si>
+  <si>
+    <t>BORJA IBANEZ</t>
+  </si>
+  <si>
+    <t>KEZHENG WANG</t>
+  </si>
+  <si>
+    <t>MICHELE EMDIN</t>
+  </si>
+  <si>
+    <t>GIANFRANCO SINAGRA</t>
+  </si>
+  <si>
+    <t>MEIYUN WANG</t>
+  </si>
+  <si>
+    <t>Y CHANDRASHEKHAR</t>
+  </si>
+  <si>
+    <t>MARTHA GROGAN</t>
+  </si>
+  <si>
+    <t>GÜNTER PILZ</t>
+  </si>
+  <si>
+    <t>ROBERT MANKA</t>
+  </si>
+  <si>
+    <t>FARZIN BEYGUI</t>
+  </si>
+  <si>
+    <t>FABAO GAO</t>
+  </si>
+  <si>
+    <t>MICHAEL K ATALAY</t>
+  </si>
+  <si>
+    <t>GREGG W STONE</t>
+  </si>
+  <si>
+    <t>ALBERT HSIAO</t>
+  </si>
+  <si>
+    <t>KHALED MANDOUR</t>
+  </si>
+  <si>
+    <t>BO LIANG</t>
+  </si>
+  <si>
+    <t>NOBUHISA HAGIWARA</t>
+  </si>
+  <si>
+    <t>BO XU</t>
+  </si>
+  <si>
+    <t>GIUSEPPE MANCIA</t>
+  </si>
+  <si>
+    <t>GERRY P MCCANN</t>
+  </si>
+  <si>
+    <t>TOMAS G NEILAN</t>
+  </si>
+  <si>
+    <t>LIANG ZHONG</t>
+  </si>
+  <si>
+    <t>SEUNG PYO LEE</t>
+  </si>
+  <si>
+    <t>COLIN BERRY</t>
+  </si>
+  <si>
+    <t>ROBERT J SIEGEL</t>
+  </si>
+  <si>
+    <t>MARC R DWECK</t>
+  </si>
+  <si>
+    <t>ANTONI BAYÉS-GENÍS</t>
+  </si>
+  <si>
+    <t>BAE YOUNG LEE</t>
+  </si>
+  <si>
+    <t>JOSÉ F RODRÍGUEZ-PALOMARES</t>
+  </si>
+  <si>
+    <t>MATTEO CAMELI</t>
+  </si>
+  <si>
+    <t>MICHEL NOUTSIAS</t>
+  </si>
+  <si>
+    <t>CHRISTIAN TEMPLIN</t>
+  </si>
+  <si>
+    <t>GIANLUCA DI BELLA</t>
+  </si>
+  <si>
+    <t>PAOLO MARINO</t>
+  </si>
+  <si>
+    <t>BERNARD COSYNS</t>
+  </si>
+  <si>
+    <t>HWAN SEOK YONG</t>
+  </si>
+  <si>
+    <t>NATALIA A TRAYANOVA</t>
+  </si>
+  <si>
+    <t>ORLANDO P SIMONETTI</t>
+  </si>
+  <si>
+    <t>PRAFULLA KERKAR</t>
+  </si>
+  <si>
+    <t>RODRIGO SALGADO</t>
+  </si>
+  <si>
+    <t>KIM A CONNELLY</t>
+  </si>
+  <si>
+    <t>HAJNALKA VAGO</t>
+  </si>
+  <si>
+    <t>VINCENT WV JADDOE</t>
+  </si>
+  <si>
+    <t>SHI JOON YOO</t>
+  </si>
+  <si>
+    <t>ARVIND NISHTALA</t>
+  </si>
+  <si>
+    <t>ARASH ARYA</t>
+  </si>
+  <si>
+    <t>PHANG BOON LIM</t>
+  </si>
+  <si>
+    <t>ARTURO EVANGELISTA</t>
+  </si>
+  <si>
+    <t>HUGH WATKINS</t>
+  </si>
+  <si>
+    <t>MATTHIAS GUTBERLET</t>
+  </si>
+  <si>
+    <t>TIM LEINER</t>
+  </si>
+  <si>
+    <t>DAVID FIRMIN</t>
+  </si>
+  <si>
+    <t>STEVEN A NIEDERER</t>
+  </si>
+  <si>
+    <t>DAVID S FRANKEL</t>
+  </si>
+  <si>
+    <t>ARNO A W ROEST</t>
+  </si>
+  <si>
+    <t>STEPHAN WINDECKER</t>
+  </si>
+  <si>
+    <t>ITSURO MORISHIMA</t>
+  </si>
+  <si>
+    <t>CHRISTOPHER A RINALDI</t>
+  </si>
+  <si>
+    <t>NADJIA KACHENOURA</t>
+  </si>
+  <si>
+    <t>DEEPAK L BHATT</t>
+  </si>
+  <si>
+    <t>HIROSHI HONDA</t>
+  </si>
+  <si>
+    <t>MENG WEI</t>
+  </si>
+  <si>
+    <t>MENGSU ZENG</t>
+  </si>
+  <si>
+    <t>THOMAS F LÜSCHER</t>
+  </si>
+  <si>
+    <t>WILLIAM W O'NEILL</t>
+  </si>
+  <si>
+    <t>NIELS VAN ROYEN</t>
+  </si>
+  <si>
+    <t>DAVID A BLUEMKE</t>
+  </si>
+  <si>
+    <t>MARCO FRANCONE</t>
+  </si>
+  <si>
+    <t>MOHAMMED Y KHANJI</t>
+  </si>
+  <si>
+    <t>ANDRÉ LA GERCHE</t>
+  </si>
+  <si>
+    <t>JOS J M WESTENBERG</t>
+  </si>
+  <si>
+    <t>RAYMOND CHING-CHEW WONG</t>
+  </si>
+  <si>
+    <t>ROB J VAN DER GEEST</t>
+  </si>
+  <si>
+    <t>ARTHUR A M WILDE</t>
+  </si>
+  <si>
+    <t>GIOVANNI DONATO AQUARO</t>
+  </si>
+  <si>
+    <t>CONNIE R BEZZINA</t>
+  </si>
+  <si>
+    <t>main specialty</t>
+  </si>
+  <si>
+    <t>Cardiology</t>
   </si>
 </sst>
 </file>
@@ -846,7 +852,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -857,6 +883,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FCB58A68-00DE-EA43-9B54-CAD687A7B0EB}" name="Table1" displayName="Table1" ref="A1:B333" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:B333" xr:uid="{FCB58A68-00DE-EA43-9B54-CAD687A7B0EB}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{42ECD9D9-5902-D148-B640-CCF29FA3559D}" name="name"/>
+    <tableColumn id="2" xr3:uid="{9F442DE4-0691-5345-9E08-6E63DB5B595B}" name="main specialty"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1146,1305 +1183,1318 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A333"/>
+  <dimension ref="A1:B333"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>20</v>
+        <v>90</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>30</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>35</v>
+        <v>123</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>39</v>
+        <v>124</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>46</v>
+        <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>11</v>
+        <v>131</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>4</v>
+        <v>134</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>103</v>
+        <v>136</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>104</v>
+        <v>137</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>106</v>
+        <v>139</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>107</v>
+        <v>140</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>109</v>
+        <v>142</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>4</v>
+        <v>145</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>113</v>
+        <v>148</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>115</v>
+        <v>150</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>116</v>
+        <v>151</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>117</v>
+        <v>152</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>118</v>
+        <v>153</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>119</v>
+        <v>154</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>121</v>
+        <v>156</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>122</v>
+        <v>157</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>124</v>
+        <v>159</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>4</v>
+        <v>162</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>127</v>
+        <v>164</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>128</v>
+        <v>165</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>131</v>
+        <v>168</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>96</v>
+        <v>169</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>132</v>
+        <v>170</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>4</v>
+        <v>172</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>134</v>
+        <v>173</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>135</v>
+        <v>174</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>136</v>
+        <v>175</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>137</v>
+        <v>176</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>57</v>
+        <v>177</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>139</v>
+        <v>180</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>140</v>
+        <v>181</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>141</v>
+        <v>182</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>142</v>
+        <v>184</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>143</v>
+        <v>185</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>4</v>
+        <v>187</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>145</v>
+        <v>188</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>18</v>
+        <v>189</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>146</v>
+        <v>190</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>147</v>
+        <v>191</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>46</v>
+        <v>192</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>148</v>
+        <v>193</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>48</v>
+        <v>194</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>149</v>
+        <v>195</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>145</v>
+        <v>196</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>150</v>
+        <v>197</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>151</v>
+        <v>198</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>152</v>
+        <v>199</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>153</v>
+        <v>200</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>154</v>
+        <v>201</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>155</v>
+        <v>202</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>157</v>
+        <v>204</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>158</v>
+        <v>205</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>160</v>
+        <v>207</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>161</v>
+        <v>208</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>162</v>
+        <v>209</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>163</v>
+        <v>210</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>164</v>
+        <v>211</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>4</v>
+        <v>212</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>165</v>
+        <v>213</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>167</v>
+        <v>215</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>168</v>
+        <v>216</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>170</v>
+        <v>218</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>171</v>
+        <v>219</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>172</v>
+        <v>220</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>173</v>
+        <v>221</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>174</v>
+        <v>222</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>175</v>
+        <v>223</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>82</v>
+        <v>224</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>176</v>
+        <v>225</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>177</v>
+        <v>226</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>175</v>
+        <v>227</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>178</v>
+        <v>228</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>144</v>
+        <v>229</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>179</v>
+        <v>230</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>154</v>
+        <v>231</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>20</v>
+        <v>232</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>180</v>
+        <v>233</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>181</v>
+        <v>234</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>182</v>
+        <v>235</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>183</v>
+        <v>236</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>184</v>
+        <v>237</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>185</v>
+        <v>238</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>186</v>
+        <v>239</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>187</v>
+        <v>240</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>188</v>
+        <v>241</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>185</v>
+        <v>242</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>189</v>
+        <v>243</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>190</v>
+        <v>244</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>191</v>
+        <v>245</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>192</v>
+        <v>246</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>193</v>
+        <v>247</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>4</v>
+        <v>248</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>81</v>
+        <v>249</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>194</v>
+        <v>250</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>195</v>
+        <v>251</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>196</v>
+        <v>252</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>59</v>
+        <v>253</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>197</v>
+        <v>254</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>198</v>
+        <v>255</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>199</v>
+        <v>256</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A259" t="s">
-        <v>162</v>
+        <v>257</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.2">
@@ -2819,5 +2869,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>